<commit_message>
NCIATWP-993: implement email tab
</commit_message>
<xml_diff>
--- a/src/assets/files/AuthorArranger Template.xlsx
+++ b/src/assets/files/AuthorArranger Template.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
   <si>
     <t>AuthorArranger Template Key</t>
   </si>
@@ -274,6 +274,24 @@
   </si>
   <si>
     <t>Street</t>
+  </si>
+  <si>
+    <t>mitchell.machiela@nih.gov</t>
+  </si>
+  <si>
+    <t>pansu@mail.nih.gov</t>
+  </si>
+  <si>
+    <t>wuye@mail.nih.gov</t>
+  </si>
+  <si>
+    <t>kai-ling.chen@nih.gov</t>
+  </si>
+  <si>
+    <t>tobiasg@mail.nih.gov</t>
+  </si>
+  <si>
+    <t>brian.park@nih.gov</t>
   </si>
 </sst>
 </file>
@@ -17344,7 +17362,9 @@
         <v>20</v>
       </c>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="H2" s="5" t="s">
         <v>39</v>
       </c>
@@ -17381,7 +17401,9 @@
         <v>20</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
         <v>37</v>
@@ -17412,6 +17434,9 @@
       </c>
       <c r="E4" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>37</v>
@@ -17461,7 +17486,9 @@
         <v>42</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="I6" s="5" t="s">
         <v>37</v>
       </c>
@@ -17494,7 +17521,9 @@
         <v>24</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="I7" s="5" t="s">
         <v>37</v>
       </c>
@@ -17530,7 +17559,9 @@
         <v>16</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="H8" s="5" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
update instructions and template
</commit_message>
<xml_diff>
--- a/src/assets/files/AuthorArranger Template.xlsx
+++ b/src/assets/files/AuthorArranger Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parkbw\Documents\nci-webtools-dceg-author-arranger\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3F135A93-BFE4-490F-8962-41C450710DE6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{56E6C512-0344-48C4-971F-D8CC9FC19403}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="56295" yWindow="8940" windowWidth="30960" windowHeight="17625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Author degree(s), if more than one separate by semicolons</t>
-  </si>
-  <si>
     <t>Miscellaneous author field to add to title page</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
   </si>
   <si>
     <t>Machiela</t>
-  </si>
-  <si>
-    <t>ScD; MPH</t>
   </si>
   <si>
     <t>Mr</t>
@@ -159,9 +153,6 @@
   </si>
   <si>
     <t>Wu</t>
-  </si>
-  <si>
-    <t>MS; PhD</t>
   </si>
   <si>
     <t>Brian</t>
@@ -293,6 +284,15 @@
   </si>
   <si>
     <t>Author institute affiliation*</t>
+  </si>
+  <si>
+    <t>Author degree(s)</t>
+  </si>
+  <si>
+    <t>MS, PhD</t>
+  </si>
+  <si>
+    <t>ScD, MPH</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
   <dimension ref="A1:XFD31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -771,71 +771,71 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -17222,55 +17222,55 @@
     </row>
     <row r="18" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -17284,7 +17284,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17321,267 +17321,267 @@
         <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -17628,31 +17628,31 @@
         <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>